<commit_message>
Update SHACL for Dataset4 : voteFromPoliticalGroup
</commit_message>
<xml_diff>
--- a/04-Dataset4_Votes/04-SHACL/Dataset4_SHACL-Shapes.xlsx
+++ b/04-Dataset4_Votes/04-SHACL/Dataset4_SHACL-Shapes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="class-based shapes" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="108">
   <si>
     <t xml:space="preserve">URI du Graphe</t>
   </si>
@@ -98,27 +98,7 @@
     <t xml:space="preserve">sh:order^^xsd:integer</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">rdfs:comment</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">^^xsd:string</t>
-    </r>
+    <t xml:space="preserve">rdfs:comment^^xsd:string</t>
   </si>
   <si>
     <t xml:space="preserve">sh:nodeKind</t>
@@ -357,6 +337,18 @@
   </si>
   <si>
     <t xml:space="preserve">Référence à des IRI qui disent « pour » / « contre » ou « abstention »</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(&lt;http://data.europarl.europa.eu/authority/votePosition/for&gt; &lt;http://data.europarl.europa.eu/authority/votePosition/foagainst&lt;http://data.europarl.europa.eu/authority/votePosition/foabstention)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eponto:voteFromPoliticalGroup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Référence au groupe politique du MEP qui a voté</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"^http://data.europarl.europa.eu/org/group/.*$"</t>
   </si>
 </sst>
 </file>
@@ -366,7 +358,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -417,13 +409,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <strike val="true"/>
@@ -518,7 +503,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -531,10 +516,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -583,31 +564,31 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -691,11 +672,11 @@
   </sheetPr>
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.4453125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.58"/>
@@ -704,7 +685,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="25.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="23.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="40.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="19.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="45.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="28.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="24.57"/>
@@ -725,11 +706,11 @@
       <c r="B2" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="2"/>
-      <c r="E2" s="4"/>
+      <c r="E2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
@@ -738,11 +719,11 @@
       <c r="B3" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="2"/>
-      <c r="E3" s="4"/>
+      <c r="E3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
@@ -751,93 +732,93 @@
       <c r="B4" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="2"/>
-      <c r="E4" s="4"/>
+      <c r="E4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-    </row>
-    <row r="8" s="9" customFormat="true" ht="50.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="9" t="s">
+      <c r="B6" s="5"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+    </row>
+    <row r="8" s="8" customFormat="true" ht="50.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="F8" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="G8" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="H8" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="I8" s="11" t="s">
+      <c r="I8" s="10" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="F9" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="G9" s="13" t="s">
+      <c r="G9" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="H9" s="12" t="s">
+      <c r="H9" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="I9" s="12" t="s">
+      <c r="I9" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="J9" s="12" t="s">
+      <c r="J9" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="K9" s="12" t="s">
+      <c r="K9" s="11" t="s">
         <v>29</v>
       </c>
     </row>
@@ -851,7 +832,7 @@
       <c r="C10" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="14"/>
+      <c r="D10" s="13"/>
       <c r="G10" s="1" t="s">
         <v>33</v>
       </c>
@@ -876,7 +857,7 @@
       <c r="C11" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D11" s="14"/>
+      <c r="D11" s="13"/>
       <c r="G11" s="1" t="s">
         <v>39</v>
       </c>
@@ -893,27 +874,27 @@
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G12" s="1"/>
-      <c r="I12" s="15"/>
+      <c r="I12" s="14"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G13" s="1"/>
-      <c r="I13" s="15"/>
+      <c r="I13" s="14"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D14" s="16"/>
+      <c r="D14" s="15"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="15"/>
+      <c r="I14" s="14"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
       <c r="G15" s="1"/>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -959,21 +940,21 @@
   </sheetPr>
   <dimension ref="A1:T1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="Q19" activeCellId="0" sqref="Q19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="40.42"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="5" min="4" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="34.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="36.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="25.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="25.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="28.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="28.86"/>
@@ -1002,7 +983,7 @@
       <c r="B2" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="Q2" s="1"/>
@@ -1014,7 +995,7 @@
       <c r="B3" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="Q3" s="1"/>
@@ -1026,169 +1007,169 @@
       <c r="B4" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="Q4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="4"/>
+      <c r="C5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="6"/>
-      <c r="O6" s="6"/>
-      <c r="P6" s="6"/>
-      <c r="Q6" s="6"/>
-      <c r="R6" s="8"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="7"/>
     </row>
     <row r="7" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G7" s="4"/>
-    </row>
-    <row r="8" s="11" customFormat="true" ht="46.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="11" t="s">
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" s="10" customFormat="true" ht="46.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="F8" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="G8" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="H8" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="I8" s="11" t="s">
+      <c r="I8" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="J8" s="11" t="s">
+      <c r="J8" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K8" s="11" t="s">
+      <c r="K8" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="L8" s="11" t="s">
+      <c r="L8" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="M8" s="11" t="s">
+      <c r="M8" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="N8" s="11" t="s">
+      <c r="N8" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="O8" s="11" t="s">
+      <c r="O8" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="P8" s="11" t="s">
+      <c r="P8" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="Q8" s="11" t="s">
+      <c r="Q8" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="R8" s="11" t="s">
+      <c r="R8" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="S8" s="11" t="s">
+      <c r="S8" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="T8" s="11" t="s">
+      <c r="T8" s="10" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="D9" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="E9" s="19" t="s">
+      <c r="E9" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="F9" s="17" t="s">
+      <c r="F9" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="G9" s="18" t="s">
+      <c r="G9" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="H9" s="18" t="s">
+      <c r="H9" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="I9" s="12" t="s">
+      <c r="I9" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="J9" s="12" t="s">
+      <c r="J9" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="K9" s="12" t="s">
+      <c r="K9" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="L9" s="18" t="s">
+      <c r="L9" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="M9" s="18" t="s">
+      <c r="M9" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="N9" s="18" t="s">
+      <c r="N9" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="O9" s="18" t="s">
+      <c r="O9" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="P9" s="18" t="s">
+      <c r="P9" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="Q9" s="18" t="s">
+      <c r="Q9" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="R9" s="13" t="s">
+      <c r="R9" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="S9" s="18" t="s">
+      <c r="S9" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="T9" s="18" t="s">
+      <c r="T9" s="17" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="10" s="20" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="20" t="s">
+    <row r="10" s="19" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="R10" s="21"/>
-      <c r="T10" s="21"/>
+      <c r="R10" s="20"/>
+      <c r="T10" s="20"/>
     </row>
     <row r="11" customFormat="false" ht="62.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="str">
@@ -1251,7 +1232,7 @@
       <c r="L12" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="R12" s="4"/>
+      <c r="R12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="str">
@@ -1291,7 +1272,7 @@
       <c r="C14" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F14" s="14" t="s">
+      <c r="F14" s="13" t="s">
         <v>94</v>
       </c>
       <c r="G14" s="1" t="n">
@@ -1306,14 +1287,14 @@
       <c r="M14" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="R14" s="4"/>
-    </row>
-    <row r="16" s="20" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="20" t="s">
+      <c r="R14" s="3"/>
+    </row>
+    <row r="16" s="19" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="R16" s="21"/>
-      <c r="T16" s="21"/>
+      <c r="R16" s="20"/>
+      <c r="T16" s="20"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="str">
@@ -1338,7 +1319,7 @@
       <c r="I17" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="J17" s="22"/>
+      <c r="J17" s="21"/>
       <c r="L17" s="0" t="s">
         <v>89</v>
       </c>
@@ -1370,7 +1351,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="96.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="str">
         <f aca="false">CONCATENATE("epsh:P",ROW(A19))</f>
         <v>epsh:P19</v>
@@ -1392,6 +1373,36 @@
       </c>
       <c r="L19" s="0" t="s">
         <v>89</v>
+      </c>
+      <c r="Q19" s="13" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="str">
+        <f aca="false">CONCATENATE("epsh:P",ROW(A20))</f>
+        <v>epsh:P20</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G20" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L20" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="R20" s="0" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Update Dataset 4 description
</commit_message>
<xml_diff>
--- a/04-Dataset4_Votes/04-SHACL/Dataset4_SHACL-Shapes.xlsx
+++ b/04-Dataset4_Votes/04-SHACL/Dataset4_SHACL-Shapes.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="149">
   <si>
     <t xml:space="preserve">Shapes URI</t>
   </si>
@@ -56,6 +56,21 @@
     <t xml:space="preserve">Votes</t>
   </si>
   <si>
+    <t xml:space="preserve">rdfs:comment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This dataset describes the votes and the position of each MEP within a given vote</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dct:modified^^xsd:date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">owl:versionInfo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">v1</t>
+  </si>
+  <si>
     <t xml:space="preserve">This sheet specifies the NodeShape with their targets, that is the sets of entities being validated</t>
   </si>
   <si>
@@ -170,6 +185,12 @@
     <t xml:space="preserve">epsh:PlenarySitting</t>
   </si>
   <si>
+    <t xml:space="preserve">Séance plénière</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plenary Sitting</t>
+  </si>
+  <si>
     <t xml:space="preserve">A plenary sitting</t>
   </si>
   <si>
@@ -179,12 +200,24 @@
     <t xml:space="preserve">epsh:VotePosition</t>
   </si>
   <si>
+    <t xml:space="preserve">Choix de vote</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vote Position</t>
+  </si>
+  <si>
     <t xml:space="preserve">A reference to a vote position (for, against, abstention)</t>
   </si>
   <si>
     <t xml:space="preserve">epsh:PoliticalGroup</t>
   </si>
   <si>
+    <t xml:space="preserve">Groupe parlementaire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Political group</t>
+  </si>
+  <si>
     <t xml:space="preserve">A reference to a Political Group</t>
   </si>
   <si>
@@ -194,6 +227,9 @@
     <t xml:space="preserve">epsh:MEP</t>
   </si>
   <si>
+    <t xml:space="preserve">MEP</t>
+  </si>
+  <si>
     <t xml:space="preserve">A reference to an MEP</t>
   </si>
   <si>
@@ -284,6 +320,9 @@
     <t xml:space="preserve">sh:name@fr</t>
   </si>
   <si>
+    <t xml:space="preserve">sh:description@en</t>
+  </si>
+  <si>
     <t xml:space="preserve">sh:minCount^^xsd:integer</t>
   </si>
   <si>
@@ -323,7 +362,10 @@
     <t xml:space="preserve">skos:prefLabel</t>
   </si>
   <si>
-    <t xml:space="preserve">preferred label</t>
+    <t xml:space="preserve">vote title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">titre du vote</t>
   </si>
   <si>
     <t xml:space="preserve">Name of the voted text (from RollCallVote.Description.Text)</t>
@@ -344,6 +386,9 @@
     <t xml:space="preserve">vote identifier</t>
   </si>
   <si>
+    <t xml:space="preserve">identifiant du vote</t>
+  </si>
+  <si>
     <t xml:space="preserve">Number of the vote (from RollCallVote.Result/@Number)</t>
   </si>
   <si>
@@ -356,13 +401,19 @@
     <t xml:space="preserve">consists of MEP vote</t>
   </si>
   <si>
+    <t xml:space="preserve">contient le vote d’un MEP</t>
+  </si>
+  <si>
     <t xml:space="preserve">Link to MEP votes in that Vote</t>
   </si>
   <si>
     <t xml:space="preserve">eponto:voteFormsPartOfPlenarySitting</t>
   </si>
   <si>
-    <t xml:space="preserve">preferred labellenary sitting</t>
+    <t xml:space="preserve">forms part of plenary sitting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fait partie d’une séance plénière</t>
   </si>
   <si>
     <t xml:space="preserve">Link to plenary sitting during which the vote took place</t>
@@ -401,6 +452,9 @@
     <t xml:space="preserve">political group</t>
   </si>
   <si>
+    <t xml:space="preserve">groupe parlementaire</t>
+  </si>
+  <si>
     <t xml:space="preserve">Link to political group to which the MEP belongs when the vote took place</t>
   </si>
   <si>
@@ -408,6 +462,9 @@
   </si>
   <si>
     <t xml:space="preserve">forms part of vote</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fait partie du vote</t>
   </si>
   <si>
     <t xml:space="preserve">Link to the vote</t>
@@ -417,9 +474,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="166" formatCode="General"/>
   </numFmts>
   <fonts count="13">
     <font>
@@ -574,7 +632,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -591,6 +649,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -659,7 +721,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -753,13 +815,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.58"/>
@@ -830,242 +892,302 @@
       <c r="E5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C6" s="3"/>
+      <c r="A6" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="2"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-    </row>
-    <row r="9" s="8" customFormat="true" ht="50.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="9" t="s">
+      <c r="A7" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="B7" s="4" t="n">
+        <v>44255</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="B8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="C8" s="2"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="B10" s="6"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+    </row>
+    <row r="12" s="9" customFormat="true" ht="50.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="B12" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="H9" s="10" t="s">
+      <c r="C12" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="I9" s="10" t="s">
+      <c r="D12" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="J9" s="10" t="s">
+      <c r="E12" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="K9" s="10" t="s">
+      <c r="F12" s="11" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="11" t="s">
+      <c r="G12" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="H12" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="J12" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="K12" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="H10" s="11" t="s">
+      <c r="C13" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="I10" s="11" t="s">
+      <c r="D13" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="J10" s="12" t="s">
+      <c r="E13" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="K10" s="12" t="s">
+      <c r="F13" s="13" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="G13" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="H13" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="I13" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="J13" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F11" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="G11" s="1" t="s">
+      <c r="K13" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="H11" s="0" t="s">
+    </row>
+    <row r="14" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="I11" s="13" t="s">
+      <c r="B14" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="K11" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="45.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="E14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="1" t="s">
+      <c r="H14" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="I14" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="J14" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F12" s="1" t="n">
+      <c r="K14" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="45.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F15" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="G15" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="I15" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K15" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="H12" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="I12" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="H13" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="I13" s="0" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="H14" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="I14" s="13"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="I15" s="0" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F16" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B16" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" s="14"/>
-      <c r="G16" s="1" t="s">
+      <c r="H16" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="I16" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="H16" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="I16" s="0" t="s">
+    </row>
+    <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G17" s="1"/>
+      <c r="B17" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F17" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H17" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="I17" s="14"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G18" s="1"/>
+      <c r="A18" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F18" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I18" s="0" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G19" s="1"/>
-    </row>
-    <row r="20" customFormat="false" ht="49.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="15"/>
+      <c r="D19" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F19" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H19" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="I19" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G20" s="1"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1074,16 +1196,25 @@
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G22" s="1"/>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="49.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="G23" s="1"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G26" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1" display="http://data.europarl.europa.eu/shapes/votes"/>
-    <hyperlink ref="D10" r:id="rId2" display="rdfs:label@fr"/>
-    <hyperlink ref="E10" r:id="rId3" display="rdfs:label@en"/>
-    <hyperlink ref="I11" r:id="rId4" display="&quot;^http://data.europarl.europa.eu/eli/dl/iPlMeeting/[0-9][0-9][0-9][0-9][0-9][0-9][0-9][0-9]/[0-9][0-9]?[0-9]?$&quot;"/>
-    <hyperlink ref="I12" r:id="rId5" display="&quot;^http://data.europarl.europa.eu/eli/dl/iPlMeeting/[0-9][0-9][0-9][0-9][0-9][0-9][0-9][0-9]/[0-9][0-9]?[0-9]?/MEP_.*$&quot;"/>
+    <hyperlink ref="D13" r:id="rId2" display="rdfs:label@fr"/>
+    <hyperlink ref="E13" r:id="rId3" display="rdfs:label@en"/>
+    <hyperlink ref="I14" r:id="rId4" display="&quot;^http://data.europarl.europa.eu/eli/dl/iPlMeeting/[0-9][0-9][0-9][0-9][0-9][0-9][0-9][0-9]/[0-9][0-9]?[0-9]?$&quot;"/>
+    <hyperlink ref="I15" r:id="rId5" display="&quot;^http://data.europarl.europa.eu/eli/dl/iPlMeeting/[0-9][0-9][0-9][0-9][0-9][0-9][0-9][0-9]/[0-9][0-9]?[0-9]?/MEP_.*$&quot;"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1100,43 +1231,43 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T20"/>
+  <dimension ref="A1:U20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="9" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="40.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="34.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="36.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="25.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="28.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="28.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="20.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="20.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="14" style="0" width="26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="26.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="41.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="34.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="28.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="34.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="36.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="25.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="18.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="28.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="28.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="20.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="20.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="15" style="0" width="26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="26.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="41.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="34.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="28.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
@@ -1148,7 +1279,7 @@
       <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
@@ -1160,178 +1291,186 @@
       <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
-      <c r="P5" s="5"/>
-      <c r="Q5" s="5"/>
-      <c r="R5" s="7"/>
-      <c r="S5" s="7"/>
-      <c r="T5" s="7"/>
+      <c r="A5" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="8"/>
+      <c r="T5" s="8"/>
+      <c r="U5" s="8"/>
     </row>
     <row r="6" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G6" s="3"/>
-    </row>
-    <row r="7" s="10" customFormat="true" ht="73.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="H7" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="I7" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="J7" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="K7" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="L7" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="M7" s="10" t="s">
+      <c r="H6" s="3"/>
+    </row>
+    <row r="7" s="11" customFormat="true" ht="73.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="N7" s="10" t="s">
+      <c r="B7" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="O7" s="10" t="s">
+      <c r="C7" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="P7" s="10" t="s">
+      <c r="D7" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="Q7" s="10" t="s">
+      <c r="E7" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="R7" s="10" t="s">
+      <c r="F7" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="G7" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="S7" s="10" t="s">
+      <c r="H7" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="T7" s="10" t="s">
+      <c r="I7" s="11" t="s">
         <v>82</v>
       </c>
+      <c r="J7" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="K7" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="L7" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="M7" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="N7" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="O7" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="P7" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q7" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="R7" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="S7" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="T7" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="U7" s="11" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" s="17" t="s">
-        <v>85</v>
+      <c r="A8" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>97</v>
       </c>
       <c r="F8" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="G8" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="H8" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="I8" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="J8" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="K8" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="L8" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="M8" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="N8" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="O8" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="P8" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q8" s="16" t="s">
-        <v>96</v>
-      </c>
-      <c r="R8" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="S8" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="T8" s="16" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="9" s="19" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="R9" s="20"/>
-      <c r="T9" s="20"/>
+      <c r="G8" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="H8" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="I8" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="K8" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="L8" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="M8" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="N8" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="O8" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="P8" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q8" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="R8" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="S8" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="T8" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="U8" s="17" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" s="20" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="S9" s="21"/>
+      <c r="U9" s="21"/>
     </row>
     <row r="10" customFormat="false" ht="62.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="str">
@@ -1339,70 +1478,76 @@
         <v>epsh:P10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>99</v>
+        <v>112</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="G10" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="H10" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="L10" s="0" t="s">
-        <v>102</v>
+        <v>114</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H10" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="M10" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q10" s="1"/>
-      <c r="T10" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>116</v>
+      </c>
+      <c r="N10" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="R10" s="1"/>
+      <c r="U10" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="str">
         <f aca="false">CONCATENATE("epsh:P",ROW(A11))</f>
         <v>epsh:P11</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>105</v>
+        <v>119</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D11" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="G11" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="H11" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="L11" s="0" t="s">
-        <v>102</v>
+        <v>120</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="H11" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="M11" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="R11" s="3"/>
+        <v>116</v>
+      </c>
+      <c r="N11" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="S11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="str">
@@ -1410,30 +1555,33 @@
         <v>epsh:P12</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D12" s="1" t="n">
         <v>3</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>110</v>
+        <v>125</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="G12" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I12" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J12" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="M12" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="L12" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="R12" s="3"/>
+      <c r="S12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="str">
@@ -1441,79 +1589,84 @@
         <v>epsh:P13</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>112</v>
+        <v>128</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D13" s="1" t="n">
         <v>4</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>113</v>
+        <v>129</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="G13" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="H13" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J13" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="L13" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="R13" s="0"/>
-    </row>
-    <row r="14" s="24" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="21" t="str">
+        <v>130</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="H13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K13" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="M13" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="S13" s="0"/>
+    </row>
+    <row r="14" s="25" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="22" t="str">
         <f aca="false">CONCATENATE("epsh:P",ROW(A14))</f>
         <v>epsh:P14</v>
       </c>
-      <c r="B14" s="21" t="s">
-        <v>115</v>
-      </c>
-      <c r="C14" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" s="22" t="n">
+      <c r="B14" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="23" t="n">
         <v>5</v>
       </c>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22" t="s">
-        <v>116</v>
-      </c>
-      <c r="G14" s="22"/>
-      <c r="H14" s="21"/>
-      <c r="I14" s="21"/>
-      <c r="J14" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="K14" s="21"/>
-      <c r="L14" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="M14" s="21"/>
-      <c r="N14" s="21"/>
-      <c r="O14" s="21"/>
-      <c r="P14" s="21"/>
-      <c r="Q14" s="21"/>
-      <c r="R14" s="23"/>
-      <c r="S14" s="21"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23" t="s">
+        <v>133</v>
+      </c>
+      <c r="H14" s="23"/>
+      <c r="I14" s="22"/>
+      <c r="J14" s="22"/>
+      <c r="K14" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="L14" s="22"/>
+      <c r="M14" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="N14" s="22"/>
+      <c r="O14" s="22"/>
+      <c r="P14" s="22"/>
+      <c r="Q14" s="22"/>
+      <c r="R14" s="22"/>
+      <c r="S14" s="24"/>
       <c r="T14" s="22"/>
-    </row>
-    <row r="16" s="19" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="19" t="s">
-        <v>117</v>
-      </c>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
-      <c r="R16" s="20"/>
-      <c r="T16" s="20"/>
+      <c r="U14" s="23"/>
+    </row>
+    <row r="16" s="20" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="20" t="s">
+        <v>134</v>
+      </c>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="21"/>
+      <c r="S16" s="21"/>
+      <c r="U16" s="21"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="str">
@@ -1521,33 +1674,36 @@
         <v>epsh:P17</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>118</v>
+        <v>135</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="D17" s="1" t="n">
         <v>1</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>119</v>
+        <v>136</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="G17" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="H17" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J17" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="L17" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="R17" s="0"/>
+        <v>136</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="H17" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K17" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="M17" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="S17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="str">
@@ -1555,34 +1711,37 @@
         <v>epsh:P18</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>121</v>
+        <v>138</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="D18" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="G18" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="H18" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J18" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="L18" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q18" s="14" t="s">
-        <v>123</v>
+        <v>72</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="H18" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I18" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K18" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="M18" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="R18" s="15" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1591,33 +1750,36 @@
         <v>epsh:P19</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>124</v>
+        <v>141</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="D19" s="1" t="n">
         <v>3</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>125</v>
+        <v>142</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="G19" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="H19" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J19" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="L19" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="R19" s="0"/>
+        <v>143</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="H19" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K19" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="M19" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="S19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="str">
@@ -1625,39 +1787,43 @@
         <v>epsh:P20</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>127</v>
+        <v>145</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="D20" s="1" t="n">
         <v>4</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>128</v>
+        <v>146</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="G20" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="H20" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I20" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="J20" s="24"/>
-      <c r="L20" s="0" t="s">
-        <v>38</v>
+        <v>147</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H20" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J20" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="K20" s="25"/>
+      <c r="M20" s="0" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1" display="http://data.europarl.europa.eu/shapes/votes"/>
-    <hyperlink ref="F8" r:id="rId2" display="sh:name@fr"/>
-    <hyperlink ref="F11" r:id="rId3" display="Number of the vote (from RollCallVote.Result/@Number)"/>
+    <hyperlink ref="F8" r:id="rId2" display="name@fr"/>
+    <hyperlink ref="G8" r:id="rId3" display="description@en"/>
+    <hyperlink ref="G11" r:id="rId4" display="Number of the vote (from RollCallVote.Result/@Number)"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>